<commit_message>
Aktualizacja notatki o kod, powodujący informacje o kradzieżach plików.
</commit_message>
<xml_diff>
--- a/.biblioteka/Lista produktów aero7 i loveair (oraz linki).xlsx
+++ b/.biblioteka/Lista produktów aero7 i loveair (oraz linki).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grzeg\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\airon24.com\.biblioteka\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45C9B29-DC5D-4C17-AB77-789999D837AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CA5820-6504-4486-BC36-3D4CDE0ED3C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D8AECA60-67FF-4262-9B25-C2369663FB7E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1" xr2:uid="{D8AECA60-67FF-4262-9B25-C2369663FB7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Produkty - lista" sheetId="2" r:id="rId1"/>
@@ -995,9 +995,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="5"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1007,11 +1004,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1339,7 +1339,7 @@
     <col min="1" max="1" width="3.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="4.42578125" style="9" customWidth="1"/>
     <col min="3" max="3" width="78.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.140625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" style="11" customWidth="1"/>
     <col min="5" max="5" width="3.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="1.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="3.28515625" style="1" customWidth="1"/>
@@ -1350,11 +1350,11 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="2:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="13"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -1575,11 +1575,11 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25"/>
     <row r="32" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="15" t="s">
         <v>217</v>
       </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="13"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="12"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25"/>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
@@ -1624,11 +1624,11 @@
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25"/>
     <row r="40" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="C40" s="11"/>
-      <c r="D40" s="13"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="12"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25"/>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
@@ -1761,11 +1761,11 @@
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25"/>
     <row r="59" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="11" t="s">
+      <c r="B59" s="15" t="s">
         <v>218</v>
       </c>
-      <c r="C59" s="11"/>
-      <c r="D59" s="13"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="12"/>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25"/>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
@@ -1884,42 +1884,42 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F18BBD9-25A5-4E7B-AA65-A1BA6A16975E}">
-  <dimension ref="A1:AD146"/>
+  <dimension ref="A1:AE146"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U46" sqref="U46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="3.5703125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="3.5703125" style="13" customWidth="1"/>
     <col min="3" max="3" width="78.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.140625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" style="11" customWidth="1"/>
     <col min="5" max="5" width="3.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="1.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="3.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="3.28515625" style="12" customWidth="1"/>
+    <col min="8" max="8" width="3.28515625" style="11" customWidth="1"/>
     <col min="9" max="9" width="52.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.140625" style="12" customWidth="1"/>
+    <col min="10" max="10" width="4.140625" style="11" customWidth="1"/>
     <col min="11" max="11" width="3.5703125" style="1" customWidth="1"/>
     <col min="12" max="12" width="1.42578125" style="2" customWidth="1"/>
     <col min="13" max="13" width="3.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="3.28515625" style="12" customWidth="1"/>
+    <col min="14" max="14" width="3.28515625" style="11" customWidth="1"/>
     <col min="15" max="15" width="74" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.140625" style="12" customWidth="1"/>
+    <col min="16" max="16" width="4.140625" style="11" customWidth="1"/>
     <col min="17" max="17" width="3.5703125" style="1" customWidth="1"/>
     <col min="18" max="18" width="1.42578125" style="2" customWidth="1"/>
     <col min="19" max="19" width="3.28515625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="3.28515625" style="12" customWidth="1"/>
+    <col min="20" max="20" width="3.28515625" style="11" customWidth="1"/>
     <col min="21" max="21" width="70.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4.140625" style="12" customWidth="1"/>
+    <col min="22" max="22" width="4.140625" style="11" customWidth="1"/>
     <col min="23" max="23" width="3.5703125" style="1" customWidth="1"/>
     <col min="24" max="24" width="1.42578125" style="2" customWidth="1"/>
     <col min="25" max="25" width="3.28515625" style="1" customWidth="1"/>
-    <col min="26" max="26" width="3.28515625" style="12" customWidth="1"/>
+    <col min="26" max="26" width="3.28515625" style="11" customWidth="1"/>
     <col min="27" max="27" width="71.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="4.140625" style="12" customWidth="1"/>
+    <col min="28" max="28" width="4.140625" style="11" customWidth="1"/>
     <col min="29" max="29" width="3.5703125" style="1" customWidth="1"/>
     <col min="30" max="30" width="1.42578125" style="2" customWidth="1"/>
     <col min="31" max="31" width="3.140625" style="1" customWidth="1"/>
@@ -1928,62 +1928,62 @@
   <sheetData>
     <row r="1" spans="2:28" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:28" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="13"/>
+      <c r="B2" s="12"/>
       <c r="C2" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="H2" s="13"/>
+      <c r="D2" s="12"/>
+      <c r="H2" s="12"/>
       <c r="I2" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="J2" s="13"/>
-      <c r="N2" s="13"/>
+      <c r="J2" s="12"/>
+      <c r="N2" s="12"/>
       <c r="O2" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="P2" s="13"/>
-      <c r="T2" s="13"/>
+      <c r="P2" s="12"/>
+      <c r="T2" s="12"/>
       <c r="U2" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="V2" s="13"/>
-      <c r="Z2" s="13"/>
+      <c r="V2" s="12"/>
+      <c r="Z2" s="12"/>
       <c r="AA2" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="AB2" s="13"/>
+      <c r="AB2" s="12"/>
     </row>
     <row r="3" spans="2:28" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="16" t="s">
         <v>221</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="H4" s="15" t="s">
+      <c r="D4" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="H4" s="16" t="s">
         <v>221</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="N4" s="15" t="s">
+      <c r="N4" s="16" t="s">
         <v>221</v>
       </c>
       <c r="O4" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="T4" s="15" t="s">
+      <c r="T4" s="16" t="s">
         <v>221</v>
       </c>
       <c r="U4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="Z4" s="12" t="s">
+      <c r="Z4" s="11" t="s">
         <v>221</v>
       </c>
       <c r="AA4" s="1" t="s">
@@ -1991,26 +1991,26 @@
       </c>
     </row>
     <row r="5" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B5" s="15"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="H5" s="15"/>
+      <c r="D5" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="H5" s="16"/>
       <c r="I5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="N5" s="15"/>
+      <c r="N5" s="16"/>
       <c r="O5" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="T5" s="15"/>
+      <c r="T5" s="16"/>
       <c r="U5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Z5" s="12" t="s">
+      <c r="Z5" s="11" t="s">
         <v>222</v>
       </c>
       <c r="AA5" s="1" t="s">
@@ -2018,22 +2018,22 @@
       </c>
     </row>
     <row r="6" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B6" s="15"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="H6" s="15"/>
+      <c r="D6" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="H6" s="16"/>
       <c r="I6" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="N6" s="15"/>
+      <c r="N6" s="16"/>
       <c r="O6" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="Z6" s="12" t="s">
+      <c r="Z6" s="11" t="s">
         <v>223</v>
       </c>
       <c r="AA6" s="1" t="s">
@@ -2041,13 +2041,13 @@
       </c>
     </row>
     <row r="7" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="T7" s="15" t="s">
+      <c r="T7" s="16" t="s">
         <v>222</v>
       </c>
       <c r="U7" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="Z7" s="12" t="s">
+      <c r="Z7" s="11" t="s">
         <v>224</v>
       </c>
       <c r="AA7" s="1" t="s">
@@ -2055,32 +2055,32 @@
       </c>
     </row>
     <row r="8" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="16" t="s">
         <v>222</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="H8" s="15" t="s">
+      <c r="D8" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="H8" s="16" t="s">
         <v>222</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="N8" s="15" t="s">
+      <c r="N8" s="16" t="s">
         <v>222</v>
       </c>
       <c r="O8" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="T8" s="15"/>
+      <c r="T8" s="16"/>
       <c r="U8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="Z8" s="12" t="s">
+      <c r="Z8" s="11" t="s">
         <v>225</v>
       </c>
       <c r="AA8" s="1" t="s">
@@ -2088,22 +2088,22 @@
       </c>
     </row>
     <row r="9" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B9" s="15"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="H9" s="15"/>
+      <c r="D9" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="H9" s="16"/>
       <c r="I9" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="N9" s="15"/>
+      <c r="N9" s="16"/>
       <c r="O9" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="Z9" s="12" t="s">
+      <c r="Z9" s="11" t="s">
         <v>226</v>
       </c>
       <c r="AA9" s="1" t="s">
@@ -2111,24 +2111,24 @@
       </c>
     </row>
     <row r="10" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B10" s="15"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="N10" s="15"/>
+      <c r="D10" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="N10" s="16"/>
       <c r="O10" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="T10" s="15" t="s">
+      <c r="T10" s="16" t="s">
         <v>223</v>
       </c>
       <c r="U10" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="Z10" s="12" t="s">
+      <c r="Z10" s="11" t="s">
         <v>227</v>
       </c>
       <c r="AA10" s="1" t="s">
@@ -2136,24 +2136,24 @@
       </c>
     </row>
     <row r="11" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B11" s="15"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="H11" s="15" t="s">
+      <c r="D11" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="H11" s="16" t="s">
         <v>223</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="T11" s="15"/>
+      <c r="T11" s="16"/>
       <c r="U11" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="Z11" s="12" t="s">
+      <c r="Z11" s="11" t="s">
         <v>228</v>
       </c>
       <c r="AA11" s="1" t="s">
@@ -2161,17 +2161,17 @@
       </c>
     </row>
     <row r="12" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="H12" s="15"/>
+      <c r="H12" s="16"/>
       <c r="I12" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="N12" s="15" t="s">
+      <c r="N12" s="16" t="s">
         <v>223</v>
       </c>
       <c r="O12" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="Z12" s="12" t="s">
+      <c r="Z12" s="11" t="s">
         <v>229</v>
       </c>
       <c r="AA12" s="1" t="s">
@@ -2179,26 +2179,26 @@
       </c>
     </row>
     <row r="13" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="16" t="s">
         <v>223</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="N13" s="15"/>
+      <c r="D13" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="N13" s="16"/>
       <c r="O13" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="T13" s="15" t="s">
+      <c r="T13" s="16" t="s">
         <v>224</v>
       </c>
       <c r="U13" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="Z13" s="12" t="s">
+      <c r="Z13" s="11" t="s">
         <v>230</v>
       </c>
       <c r="AA13" s="1" t="s">
@@ -2206,28 +2206,28 @@
       </c>
     </row>
     <row r="14" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B14" s="15"/>
+      <c r="B14" s="16"/>
       <c r="C14" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="H14" s="15" t="s">
+      <c r="D14" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="H14" s="16" t="s">
         <v>224</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="N14" s="15"/>
+      <c r="N14" s="16"/>
       <c r="O14" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="T14" s="15"/>
+      <c r="T14" s="16"/>
       <c r="U14" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="Z14" s="12" t="s">
+      <c r="Z14" s="11" t="s">
         <v>231</v>
       </c>
       <c r="AA14" s="1" t="s">
@@ -2235,18 +2235,18 @@
       </c>
     </row>
     <row r="15" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B15" s="15"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="H15" s="15"/>
+      <c r="D15" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="H15" s="16"/>
       <c r="I15" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="Z15" s="12" t="s">
+      <c r="Z15" s="11" t="s">
         <v>232</v>
       </c>
       <c r="AA15" s="1" t="s">
@@ -2254,26 +2254,26 @@
       </c>
     </row>
     <row r="16" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B16" s="15"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="N16" s="15" t="s">
+      <c r="D16" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="N16" s="16" t="s">
         <v>224</v>
       </c>
       <c r="O16" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="T16" s="15" t="s">
+      <c r="T16" s="16" t="s">
         <v>225</v>
       </c>
       <c r="U16" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="Z16" s="12" t="s">
+      <c r="Z16" s="11" t="s">
         <v>233</v>
       </c>
       <c r="AA16" s="1" t="s">
@@ -2281,28 +2281,28 @@
       </c>
     </row>
     <row r="17" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B17" s="15"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="H17" s="15" t="s">
+      <c r="D17" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="H17" s="16" t="s">
         <v>225</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="N17" s="15"/>
+      <c r="N17" s="16"/>
       <c r="O17" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="T17" s="15"/>
+      <c r="T17" s="16"/>
       <c r="U17" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="Z17" s="12" t="s">
+      <c r="Z17" s="11" t="s">
         <v>234</v>
       </c>
       <c r="AA17" s="1" t="s">
@@ -2310,15 +2310,15 @@
       </c>
     </row>
     <row r="18" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="H18" s="15"/>
+      <c r="H18" s="16"/>
       <c r="I18" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="N18" s="15"/>
+      <c r="N18" s="16"/>
       <c r="O18" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="Z18" s="12" t="s">
+      <c r="Z18" s="11" t="s">
         <v>235</v>
       </c>
       <c r="AA18" s="1" t="s">
@@ -2326,19 +2326,19 @@
       </c>
     </row>
     <row r="19" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="16" t="s">
         <v>224</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="T19" s="15" t="s">
+      <c r="T19" s="16" t="s">
         <v>226</v>
       </c>
       <c r="U19" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="Z19" s="12" t="s">
+      <c r="Z19" s="11" t="s">
         <v>236</v>
       </c>
       <c r="AA19" s="1" t="s">
@@ -2346,24 +2346,24 @@
       </c>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B20" s="15"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="N20" s="15" t="s">
+      <c r="D20" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="N20" s="16" t="s">
         <v>225</v>
       </c>
       <c r="O20" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="T20" s="15"/>
+      <c r="T20" s="16"/>
       <c r="U20" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="Z20" s="12" t="s">
+      <c r="Z20" s="11" t="s">
         <v>237</v>
       </c>
       <c r="AA20" s="1" t="s">
@@ -2371,18 +2371,18 @@
       </c>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B21" s="15"/>
+      <c r="B21" s="16"/>
       <c r="C21" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="N21" s="15"/>
+      <c r="D21" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="N21" s="16"/>
       <c r="O21" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="Z21" s="12" t="s">
+      <c r="Z21" s="11" t="s">
         <v>238</v>
       </c>
       <c r="AA21" s="1" t="s">
@@ -2390,20 +2390,20 @@
       </c>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B22" s="15"/>
+      <c r="B22" s="16"/>
       <c r="C22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="T22" s="15" t="s">
+      <c r="D22" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="T22" s="16" t="s">
         <v>227</v>
       </c>
       <c r="U22" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="Z22" s="12" t="s">
+      <c r="Z22" s="11" t="s">
         <v>239</v>
       </c>
       <c r="AA22" s="1" t="s">
@@ -2411,24 +2411,24 @@
       </c>
     </row>
     <row r="23" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B23" s="15"/>
+      <c r="B23" s="16"/>
       <c r="C23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="N23" s="15" t="s">
+      <c r="D23" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="N23" s="16" t="s">
         <v>226</v>
       </c>
       <c r="O23" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="T23" s="15"/>
+      <c r="T23" s="16"/>
       <c r="U23" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="Z23" s="12" t="s">
+      <c r="Z23" s="11" t="s">
         <v>240</v>
       </c>
       <c r="AA23" s="1" t="s">
@@ -2436,11 +2436,11 @@
       </c>
     </row>
     <row r="24" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="N24" s="15"/>
+      <c r="N24" s="16"/>
       <c r="O24" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Z24" s="12" t="s">
+      <c r="Z24" s="11" t="s">
         <v>241</v>
       </c>
       <c r="AA24" s="1" t="s">
@@ -2448,19 +2448,19 @@
       </c>
     </row>
     <row r="25" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="16" t="s">
         <v>225</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="T25" s="15" t="s">
+      <c r="T25" s="16" t="s">
         <v>228</v>
       </c>
       <c r="U25" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="Z25" s="12" t="s">
+      <c r="Z25" s="11" t="s">
         <v>242</v>
       </c>
       <c r="AA25" s="1" t="s">
@@ -2468,24 +2468,24 @@
       </c>
     </row>
     <row r="26" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B26" s="15"/>
+      <c r="B26" s="16"/>
       <c r="C26" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D26" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="N26" s="15" t="s">
+      <c r="D26" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="N26" s="16" t="s">
         <v>227</v>
       </c>
       <c r="O26" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="T26" s="15"/>
+      <c r="T26" s="16"/>
       <c r="U26" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="Z26" s="12" t="s">
+      <c r="Z26" s="11" t="s">
         <v>243</v>
       </c>
       <c r="AA26" s="1" t="s">
@@ -2493,18 +2493,18 @@
       </c>
     </row>
     <row r="27" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B27" s="15"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="N27" s="15"/>
+      <c r="D27" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="N27" s="16"/>
       <c r="O27" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="Z27" s="12" t="s">
+      <c r="Z27" s="11" t="s">
         <v>244</v>
       </c>
       <c r="AA27" s="1" t="s">
@@ -2512,17 +2512,17 @@
       </c>
     </row>
     <row r="28" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="N28" s="15"/>
+      <c r="N28" s="16"/>
       <c r="O28" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="T28" s="15" t="s">
+      <c r="T28" s="16" t="s">
         <v>229</v>
       </c>
       <c r="U28" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="Z28" s="12" t="s">
+      <c r="Z28" s="11" t="s">
         <v>245</v>
       </c>
       <c r="AA28" s="1" t="s">
@@ -2530,20 +2530,20 @@
       </c>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="16" t="s">
         <v>226</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="T29" s="15"/>
+      <c r="D29" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="T29" s="16"/>
       <c r="U29" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="Z29" s="12" t="s">
+      <c r="Z29" s="11" t="s">
         <v>246</v>
       </c>
       <c r="AA29" s="1" t="s">
@@ -2551,20 +2551,20 @@
       </c>
     </row>
     <row r="30" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B30" s="15"/>
+      <c r="B30" s="16"/>
       <c r="C30" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="N30" s="15" t="s">
+      <c r="D30" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="N30" s="16" t="s">
         <v>228</v>
       </c>
       <c r="O30" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="Z30" s="12" t="s">
+      <c r="Z30" s="11" t="s">
         <v>247</v>
       </c>
       <c r="AA30" s="1" t="s">
@@ -2572,24 +2572,24 @@
       </c>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B31" s="15"/>
+      <c r="B31" s="16"/>
       <c r="C31" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="N31" s="15"/>
+      <c r="D31" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="N31" s="16"/>
       <c r="O31" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="T31" s="15" t="s">
+      <c r="T31" s="16" t="s">
         <v>230</v>
       </c>
       <c r="U31" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="Z31" s="12" t="s">
+      <c r="Z31" s="11" t="s">
         <v>248</v>
       </c>
       <c r="AA31" s="1" t="s">
@@ -2597,22 +2597,22 @@
       </c>
     </row>
     <row r="32" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B32" s="15"/>
+      <c r="B32" s="16"/>
       <c r="C32" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="N32" s="15"/>
+      <c r="D32" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="N32" s="16"/>
       <c r="O32" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="T32" s="15"/>
+      <c r="T32" s="16"/>
       <c r="U32" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="Z32" s="12" t="s">
+      <c r="Z32" s="11" t="s">
         <v>249</v>
       </c>
       <c r="AA32" s="1" t="s">
@@ -2620,22 +2620,22 @@
       </c>
     </row>
     <row r="33" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B33" s="15"/>
+      <c r="B33" s="16"/>
       <c r="C33" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D33" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="34" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="N34" s="15" t="s">
+      <c r="N34" s="16" t="s">
         <v>229</v>
       </c>
       <c r="O34" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="T34" s="15" t="s">
+      <c r="T34" s="16" t="s">
         <v>231</v>
       </c>
       <c r="U34" s="6" t="s">
@@ -2643,43 +2643,43 @@
       </c>
     </row>
     <row r="35" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="16" t="s">
         <v>227</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="N35" s="15"/>
+      <c r="N35" s="16"/>
       <c r="O35" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="T35" s="15"/>
+      <c r="T35" s="16"/>
       <c r="U35" s="1" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="36" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B36" s="15"/>
+      <c r="B36" s="16"/>
       <c r="C36" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D36" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="N36" s="15"/>
+      <c r="D36" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="N36" s="16"/>
       <c r="O36" s="1" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="37" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B37" s="15"/>
+      <c r="B37" s="16"/>
       <c r="C37" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D37" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="T37" s="15" t="s">
+      <c r="D37" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="T37" s="16" t="s">
         <v>232</v>
       </c>
       <c r="U37" s="4" t="s">
@@ -2687,45 +2687,45 @@
       </c>
     </row>
     <row r="38" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B38" s="15"/>
+      <c r="B38" s="16"/>
       <c r="C38" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D38" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="N38" s="15" t="s">
+      <c r="D38" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="N38" s="16" t="s">
         <v>230</v>
       </c>
       <c r="O38" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="T38" s="15"/>
+      <c r="T38" s="16"/>
       <c r="U38" s="1" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="39" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B39" s="15"/>
+      <c r="B39" s="16"/>
       <c r="C39" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D39" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="N39" s="15"/>
+      <c r="D39" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="N39" s="16"/>
       <c r="O39" s="1" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="40" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="N40" s="15"/>
+      <c r="N40" s="16"/>
       <c r="O40" s="1" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="41" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="16" t="s">
         <v>228</v>
       </c>
       <c r="C41" s="4" t="s">
@@ -2733,11 +2733,11 @@
       </c>
     </row>
     <row r="42" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B42" s="15"/>
+      <c r="B42" s="16"/>
       <c r="C42" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="N42" s="15" t="s">
+      <c r="N42" s="16" t="s">
         <v>231</v>
       </c>
       <c r="O42" s="4" t="s">
@@ -2745,13 +2745,13 @@
       </c>
     </row>
     <row r="43" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="N43" s="15"/>
+      <c r="N43" s="16"/>
       <c r="O43" s="1" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="44" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="16" t="s">
         <v>229</v>
       </c>
       <c r="C44" s="4" t="s">
@@ -2759,11 +2759,11 @@
       </c>
     </row>
     <row r="45" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B45" s="15"/>
+      <c r="B45" s="16"/>
       <c r="C45" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="N45" s="15" t="s">
+      <c r="N45" s="16" t="s">
         <v>232</v>
       </c>
       <c r="O45" s="4" t="s">
@@ -2771,13 +2771,13 @@
       </c>
     </row>
     <row r="46" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="N46" s="15"/>
+      <c r="N46" s="16"/>
       <c r="O46" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="47" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="16" t="s">
         <v>230</v>
       </c>
       <c r="C47" s="4" t="s">
@@ -2785,11 +2785,11 @@
       </c>
     </row>
     <row r="48" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B48" s="15"/>
+      <c r="B48" s="16"/>
       <c r="C48" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="N48" s="15" t="s">
+      <c r="N48" s="16" t="s">
         <v>233</v>
       </c>
       <c r="O48" s="4" t="s">
@@ -2797,13 +2797,13 @@
       </c>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="N49" s="15"/>
+      <c r="N49" s="16"/>
       <c r="O49" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B50" s="15" t="s">
+      <c r="B50" s="16" t="s">
         <v>231</v>
       </c>
       <c r="C50" s="4" t="s">
@@ -2811,14 +2811,14 @@
       </c>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B51" s="15"/>
+      <c r="B51" s="16"/>
       <c r="C51" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D51" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="N51" s="15" t="s">
+      <c r="D51" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="N51" s="16" t="s">
         <v>234</v>
       </c>
       <c r="O51" s="4" t="s">
@@ -2826,36 +2826,36 @@
       </c>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B52" s="15"/>
+      <c r="B52" s="16"/>
       <c r="C52" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D52" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="N52" s="15"/>
+      <c r="D52" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="N52" s="16"/>
       <c r="O52" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B53" s="15"/>
+      <c r="B53" s="16"/>
       <c r="C53" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D53" s="12" t="s">
+      <c r="D53" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B54" s="15"/>
+      <c r="B54" s="16"/>
       <c r="C54" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D54" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="N54" s="15" t="s">
+      <c r="D54" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="N54" s="16" t="s">
         <v>235</v>
       </c>
       <c r="O54" s="4" t="s">
@@ -2863,36 +2863,36 @@
       </c>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B55" s="15"/>
+      <c r="B55" s="16"/>
       <c r="C55" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D55" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="N55" s="15"/>
+      <c r="D55" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="N55" s="16"/>
       <c r="O55" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B56" s="15"/>
+      <c r="B56" s="16"/>
       <c r="C56" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D56" s="12" t="s">
+      <c r="D56" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B57" s="15"/>
+      <c r="B57" s="16"/>
       <c r="C57" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D57" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="N57" s="15" t="s">
+      <c r="D57" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="N57" s="16" t="s">
         <v>236</v>
       </c>
       <c r="O57" s="4" t="s">
@@ -2900,13 +2900,13 @@
       </c>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="N58" s="15"/>
+      <c r="N58" s="16"/>
       <c r="O58" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B59" s="15" t="s">
+      <c r="B59" s="16" t="s">
         <v>232</v>
       </c>
       <c r="C59" s="4" t="s">
@@ -2914,44 +2914,44 @@
       </c>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B60" s="15"/>
+      <c r="B60" s="16"/>
       <c r="C60" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D60" s="12" t="s">
+      <c r="D60" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B61" s="15"/>
+      <c r="B61" s="16"/>
       <c r="C61" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D61" s="12" t="s">
+      <c r="D61" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B62" s="15"/>
+      <c r="B62" s="16"/>
       <c r="C62" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D62" s="12" t="s">
+      <c r="D62" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B63" s="15"/>
+      <c r="B63" s="16"/>
       <c r="C63" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D63" s="12" t="s">
+      <c r="D63" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.25"/>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="15" t="s">
+      <c r="B65" s="16" t="s">
         <v>233</v>
       </c>
       <c r="C65" s="4" t="s">
@@ -2959,44 +2959,44 @@
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B66" s="15"/>
+      <c r="B66" s="16"/>
       <c r="C66" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D66" s="12" t="s">
+      <c r="D66" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="15"/>
+      <c r="B67" s="16"/>
       <c r="C67" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D67" s="12" t="s">
+      <c r="D67" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="15"/>
+      <c r="B68" s="16"/>
       <c r="C68" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D68" s="12" t="s">
+      <c r="D68" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B69" s="15"/>
+      <c r="B69" s="16"/>
       <c r="C69" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D69" s="12" t="s">
+      <c r="D69" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25"/>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="15" t="s">
+      <c r="B71" s="16" t="s">
         <v>234</v>
       </c>
       <c r="C71" s="4" t="s">
@@ -3004,44 +3004,44 @@
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B72" s="15"/>
+      <c r="B72" s="16"/>
       <c r="C72" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D72" s="12" t="s">
+      <c r="D72" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="15"/>
+      <c r="B73" s="16"/>
       <c r="C73" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D73" s="12" t="s">
+      <c r="D73" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B74" s="15"/>
+      <c r="B74" s="16"/>
       <c r="C74" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D74" s="12" t="s">
+      <c r="D74" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="15"/>
+      <c r="B75" s="16"/>
       <c r="C75" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D75" s="12" t="s">
+      <c r="D75" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25"/>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B77" s="15" t="s">
+      <c r="B77" s="16" t="s">
         <v>235</v>
       </c>
       <c r="C77" s="4" t="s">
@@ -3049,44 +3049,44 @@
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B78" s="15"/>
+      <c r="B78" s="16"/>
       <c r="C78" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="D78" s="12" t="s">
+      <c r="D78" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B79" s="15"/>
+      <c r="B79" s="16"/>
       <c r="C79" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D79" s="12" t="s">
+      <c r="D79" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B80" s="15"/>
+      <c r="B80" s="16"/>
       <c r="C80" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D80" s="12" t="s">
+      <c r="D80" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B81" s="15"/>
+      <c r="B81" s="16"/>
       <c r="C81" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D81" s="12" t="s">
+      <c r="D81" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.25"/>
     <row r="83" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B83" s="15" t="s">
+      <c r="B83" s="16" t="s">
         <v>236</v>
       </c>
       <c r="C83" s="4" t="s">
@@ -3094,44 +3094,44 @@
       </c>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B84" s="15"/>
+      <c r="B84" s="16"/>
       <c r="C84" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D84" s="12" t="s">
+      <c r="D84" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B85" s="15"/>
+      <c r="B85" s="16"/>
       <c r="C85" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D85" s="12" t="s">
+      <c r="D85" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B86" s="15"/>
+      <c r="B86" s="16"/>
       <c r="C86" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D86" s="12" t="s">
+      <c r="D86" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B87" s="15"/>
+      <c r="B87" s="16"/>
       <c r="C87" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D87" s="12" t="s">
+      <c r="D87" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.25"/>
     <row r="89" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B89" s="15" t="s">
+      <c r="B89" s="16" t="s">
         <v>237</v>
       </c>
       <c r="C89" s="4" t="s">
@@ -3139,44 +3139,44 @@
       </c>
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B90" s="15"/>
+      <c r="B90" s="16"/>
       <c r="C90" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="D90" s="12" t="s">
+      <c r="D90" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B91" s="15"/>
+      <c r="B91" s="16"/>
       <c r="C91" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D91" s="12" t="s">
+      <c r="D91" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B92" s="15"/>
+      <c r="B92" s="16"/>
       <c r="C92" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D92" s="12" t="s">
+      <c r="D92" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B93" s="15"/>
+      <c r="B93" s="16"/>
       <c r="C93" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D93" s="12" t="s">
+      <c r="D93" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.25"/>
     <row r="95" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B95" s="15" t="s">
+      <c r="B95" s="16" t="s">
         <v>238</v>
       </c>
       <c r="C95" s="4" t="s">
@@ -3184,26 +3184,26 @@
       </c>
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B96" s="15"/>
+      <c r="B96" s="16"/>
       <c r="C96" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D96" s="12" t="s">
+      <c r="D96" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B97" s="15"/>
+      <c r="B97" s="16"/>
       <c r="C97" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D97" s="12" t="s">
+      <c r="D97" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25"/>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B99" s="15" t="s">
+      <c r="B99" s="16" t="s">
         <v>239</v>
       </c>
       <c r="C99" s="4" t="s">
@@ -3211,44 +3211,44 @@
       </c>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B100" s="15"/>
+      <c r="B100" s="16"/>
       <c r="C100" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="D100" s="12" t="s">
+      <c r="D100" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B101" s="15"/>
+      <c r="B101" s="16"/>
       <c r="C101" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D101" s="12" t="s">
+      <c r="D101" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B102" s="15"/>
+      <c r="B102" s="16"/>
       <c r="C102" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D102" s="12" t="s">
+      <c r="D102" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B103" s="15"/>
+      <c r="B103" s="16"/>
       <c r="C103" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D103" s="12" t="s">
+      <c r="D103" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.25"/>
     <row r="105" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B105" s="15" t="s">
+      <c r="B105" s="16" t="s">
         <v>240</v>
       </c>
       <c r="C105" s="4" t="s">
@@ -3256,44 +3256,44 @@
       </c>
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B106" s="15"/>
+      <c r="B106" s="16"/>
       <c r="C106" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="D106" s="12" t="s">
+      <c r="D106" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="107" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B107" s="15"/>
+      <c r="B107" s="16"/>
       <c r="C107" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D107" s="12" t="s">
+      <c r="D107" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="108" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B108" s="15"/>
+      <c r="B108" s="16"/>
       <c r="C108" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D108" s="12" t="s">
+      <c r="D108" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="109" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B109" s="15"/>
+      <c r="B109" s="16"/>
       <c r="C109" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D109" s="12" t="s">
+      <c r="D109" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.25"/>
     <row r="111" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B111" s="15" t="s">
+      <c r="B111" s="16" t="s">
         <v>241</v>
       </c>
       <c r="C111" s="4" t="s">
@@ -3301,44 +3301,44 @@
       </c>
     </row>
     <row r="112" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B112" s="15"/>
+      <c r="B112" s="16"/>
       <c r="C112" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D112" s="12" t="s">
+      <c r="D112" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="113" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B113" s="15"/>
+      <c r="B113" s="16"/>
       <c r="C113" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D113" s="12" t="s">
+      <c r="D113" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="114" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B114" s="15"/>
+      <c r="B114" s="16"/>
       <c r="C114" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D114" s="12" t="s">
+      <c r="D114" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="115" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B115" s="15"/>
+      <c r="B115" s="16"/>
       <c r="C115" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D115" s="12" t="s">
+      <c r="D115" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="116" spans="2:4" x14ac:dyDescent="0.25"/>
     <row r="117" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B117" s="15" t="s">
+      <c r="B117" s="16" t="s">
         <v>242</v>
       </c>
       <c r="C117" s="4" t="s">
@@ -3346,44 +3346,44 @@
       </c>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B118" s="15"/>
+      <c r="B118" s="16"/>
       <c r="C118" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D118" s="12" t="s">
+      <c r="D118" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="119" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B119" s="15"/>
+      <c r="B119" s="16"/>
       <c r="C119" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D119" s="12" t="s">
+      <c r="D119" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="120" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B120" s="15"/>
+      <c r="B120" s="16"/>
       <c r="C120" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D120" s="12" t="s">
+      <c r="D120" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B121" s="15"/>
+      <c r="B121" s="16"/>
       <c r="C121" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D121" s="12" t="s">
+      <c r="D121" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="122" spans="2:4" x14ac:dyDescent="0.25"/>
     <row r="123" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B123" s="15" t="s">
+      <c r="B123" s="16" t="s">
         <v>243</v>
       </c>
       <c r="C123" s="4" t="s">
@@ -3391,44 +3391,44 @@
       </c>
     </row>
     <row r="124" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B124" s="15"/>
+      <c r="B124" s="16"/>
       <c r="C124" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="D124" s="12" t="s">
+      <c r="D124" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="125" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B125" s="15"/>
+      <c r="B125" s="16"/>
       <c r="C125" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D125" s="12" t="s">
+      <c r="D125" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="126" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B126" s="15"/>
+      <c r="B126" s="16"/>
       <c r="C126" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D126" s="12" t="s">
+      <c r="D126" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="127" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B127" s="15"/>
+      <c r="B127" s="16"/>
       <c r="C127" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D127" s="12" t="s">
+      <c r="D127" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="128" spans="2:4" x14ac:dyDescent="0.25"/>
     <row r="129" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B129" s="15" t="s">
+      <c r="B129" s="16" t="s">
         <v>244</v>
       </c>
       <c r="C129" s="4" t="s">
@@ -3436,26 +3436,26 @@
       </c>
     </row>
     <row r="130" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B130" s="15"/>
+      <c r="B130" s="16"/>
       <c r="C130" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="D130" s="12" t="s">
+      <c r="D130" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="131" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B131" s="15"/>
+      <c r="B131" s="16"/>
       <c r="C131" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D131" s="12" t="s">
+      <c r="D131" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="132" spans="2:4" x14ac:dyDescent="0.25"/>
     <row r="133" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B133" s="15" t="s">
+      <c r="B133" s="16" t="s">
         <v>245</v>
       </c>
       <c r="C133" s="4" t="s">
@@ -3463,38 +3463,38 @@
       </c>
     </row>
     <row r="134" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B134" s="15"/>
+      <c r="B134" s="16"/>
       <c r="C134" s="7" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="135" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B135" s="15"/>
+      <c r="B135" s="16"/>
       <c r="C135" s="7" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="136" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B136" s="15"/>
+      <c r="B136" s="16"/>
       <c r="C136" s="1" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="137" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B137" s="15"/>
+      <c r="B137" s="16"/>
       <c r="C137" s="1" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="138" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B138" s="15"/>
+      <c r="B138" s="16"/>
       <c r="C138" s="1" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="139" spans="2:4" x14ac:dyDescent="0.25"/>
     <row r="140" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B140" s="15" t="s">
+      <c r="B140" s="16" t="s">
         <v>246</v>
       </c>
       <c r="C140" s="4" t="s">
@@ -3502,17 +3502,17 @@
       </c>
     </row>
     <row r="141" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B141" s="15"/>
+      <c r="B141" s="16"/>
       <c r="C141" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="D141" s="12" t="s">
+      <c r="D141" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="142" spans="2:4" x14ac:dyDescent="0.25"/>
     <row r="143" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B143" s="15" t="s">
+      <c r="B143" s="16" t="s">
         <v>247</v>
       </c>
       <c r="C143" s="4" t="s">
@@ -3520,11 +3520,11 @@
       </c>
     </row>
     <row r="144" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B144" s="15"/>
-      <c r="C144" s="16" t="s">
+      <c r="B144" s="16"/>
+      <c r="C144" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="D144" s="12" t="s">
+      <c r="D144" s="11" t="s">
         <v>281</v>
       </c>
     </row>
@@ -3532,39 +3532,17 @@
     <row r="146" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="T4:T5"/>
-    <mergeCell ref="T22:T23"/>
-    <mergeCell ref="T19:T20"/>
-    <mergeCell ref="T16:T17"/>
-    <mergeCell ref="T13:T14"/>
-    <mergeCell ref="T10:T11"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="N20:N21"/>
-    <mergeCell ref="N16:N18"/>
-    <mergeCell ref="N12:N14"/>
-    <mergeCell ref="N8:N10"/>
-    <mergeCell ref="N4:N6"/>
-    <mergeCell ref="T37:T38"/>
-    <mergeCell ref="T34:T35"/>
-    <mergeCell ref="T31:T32"/>
-    <mergeCell ref="T28:T29"/>
-    <mergeCell ref="T25:T26"/>
-    <mergeCell ref="N42:N43"/>
-    <mergeCell ref="N38:N40"/>
-    <mergeCell ref="N34:N36"/>
-    <mergeCell ref="N30:N32"/>
-    <mergeCell ref="N26:N28"/>
-    <mergeCell ref="N23:N24"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="N57:N58"/>
-    <mergeCell ref="N54:N55"/>
-    <mergeCell ref="N51:N52"/>
-    <mergeCell ref="N48:N49"/>
-    <mergeCell ref="N45:N46"/>
+    <mergeCell ref="B77:B81"/>
+    <mergeCell ref="B105:B109"/>
+    <mergeCell ref="B99:B103"/>
+    <mergeCell ref="B95:B97"/>
+    <mergeCell ref="B89:B93"/>
+    <mergeCell ref="B83:B87"/>
+    <mergeCell ref="B65:B69"/>
+    <mergeCell ref="B59:B63"/>
+    <mergeCell ref="B50:B57"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B44:B45"/>
     <mergeCell ref="B8:B11"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="B143:B144"/>
@@ -3581,17 +3559,39 @@
     <mergeCell ref="B19:B23"/>
     <mergeCell ref="B13:B17"/>
     <mergeCell ref="B71:B75"/>
-    <mergeCell ref="B65:B69"/>
-    <mergeCell ref="B59:B63"/>
-    <mergeCell ref="B50:B57"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B105:B109"/>
-    <mergeCell ref="B99:B103"/>
-    <mergeCell ref="B95:B97"/>
-    <mergeCell ref="B89:B93"/>
-    <mergeCell ref="B83:B87"/>
-    <mergeCell ref="B77:B81"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="N57:N58"/>
+    <mergeCell ref="N54:N55"/>
+    <mergeCell ref="N51:N52"/>
+    <mergeCell ref="N48:N49"/>
+    <mergeCell ref="N45:N46"/>
+    <mergeCell ref="N23:N24"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="N42:N43"/>
+    <mergeCell ref="N38:N40"/>
+    <mergeCell ref="N34:N36"/>
+    <mergeCell ref="N30:N32"/>
+    <mergeCell ref="N26:N28"/>
+    <mergeCell ref="T37:T38"/>
+    <mergeCell ref="T34:T35"/>
+    <mergeCell ref="T31:T32"/>
+    <mergeCell ref="T28:T29"/>
+    <mergeCell ref="T25:T26"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="N16:N18"/>
+    <mergeCell ref="N12:N14"/>
+    <mergeCell ref="N8:N10"/>
+    <mergeCell ref="N4:N6"/>
+    <mergeCell ref="T4:T5"/>
+    <mergeCell ref="T22:T23"/>
+    <mergeCell ref="T19:T20"/>
+    <mergeCell ref="T16:T17"/>
+    <mergeCell ref="T13:T14"/>
+    <mergeCell ref="T10:T11"/>
+    <mergeCell ref="T7:T8"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>